<commit_message>
Fix: Add employee data and latest app updates with instructions
</commit_message>
<xml_diff>
--- a/data/employees.xlsx
+++ b/data/employees.xlsx
@@ -561,11 +561,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
+          <t>Gewitter</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -596,7 +596,7 @@
           <t>Gewitter</t>
         </is>
       </c>
-      <c r="G5" t="b">
+      <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">

</xml_diff>